<commit_message>
- Actualizacion de Templates FluNet
</commit_message>
<xml_diff>
--- a/Template/Export/Bitacora_B1_17.xlsx
+++ b/Template/Export/Bitacora_B1_17.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Template\Export\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
@@ -164,7 +159,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -216,7 +211,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -410,7 +405,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -425,7 +420,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>

</xml_diff>